<commit_message>
tabelas atualizadas, portugal, europa e fora da europa/ Graficos a funcionar
</commit_message>
<xml_diff>
--- a/Docs/Partidos.xlsx
+++ b/Docs/Partidos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eduardomaio/Vot-metro-A-Volta-a-Portugal-em-Elei-es/Docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eduardomaio/Desktop/Votometro-A-Volta-a-Portugal-em-Eleicoes/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC8B4D7-F2D3-5848-932A-11972DE76D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A432C923-5A2B-B14A-B2D7-170C3B38AF7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="29040" windowHeight="15840" xr2:uid="{8838E7B8-CBE2-46B9-A0E3-9A815B1E9823}"/>
   </bookViews>
@@ -752,8 +752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA66F45C-4312-462E-BED8-B9429D627A4D}">
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>